<commit_message>
fixed #731 FlixelRL-731 アンロック管理の実装
</commit_message>
<xml_diff>
--- a/docs/achievement.xlsx
+++ b/docs/achievement.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58">
   <si>
     <t>id</t>
   </si>
@@ -119,7 +119,10 @@
     <t>ナイトメアLv1撃破</t>
   </si>
   <si>
-    <t>nightmare</t>
+    <t>enemy</t>
+  </si>
+  <si>
+    <t>NIGHTMARE</t>
   </si>
   <si>
     <t>ナイトメアを倒そう</t>
@@ -128,22 +131,43 @@
     <t>ナイトメアLv2撃破</t>
   </si>
   <si>
+    <t>FIRE_DEMON</t>
+  </si>
+  <si>
     <t>ナイトメアLv3撃破</t>
   </si>
   <si>
+    <t>WATER_DEMON</t>
+  </si>
+  <si>
     <t>ナイトメアLv4撃破</t>
   </si>
   <si>
+    <t>EARTH_DEMON</t>
+  </si>
+  <si>
     <t>ナイトメアLv5撃破</t>
   </si>
   <si>
+    <t>WIND_DEMON</t>
+  </si>
+  <si>
     <t>ナイトメアLv6撃破</t>
   </si>
   <si>
+    <t>POISON_DEMON</t>
+  </si>
+  <si>
     <t>ナイトメアLv7撃破</t>
   </si>
   <si>
+    <t>SHADOW_DEMON</t>
+  </si>
+  <si>
     <t>ナイトメアLv8撃破</t>
+  </si>
+  <si>
+    <t>ICE_DEMON</t>
   </si>
   <si>
     <t>空腹で倒れた</t>
@@ -1529,8 +1553,8 @@
   <cols>
     <col min="1" max="1" width="3.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.0469" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.125" style="1" customWidth="1"/>
     <col min="5" max="5" width="6.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="6.5" style="1" customWidth="1"/>
     <col min="7" max="7" width="26.8438" style="1" customWidth="1"/>
@@ -1876,13 +1900,13 @@
       <c r="C18" t="s" s="4">
         <v>35</v>
       </c>
-      <c r="D18" s="4">
-        <v>1</v>
+      <c r="D18" t="s" s="4">
+        <v>36</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" t="s" s="4">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" ht="20" customHeight="1">
@@ -1890,18 +1914,18 @@
         <v>17</v>
       </c>
       <c r="B19" t="s" s="4">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s" s="4">
         <v>35</v>
       </c>
-      <c r="D19" s="4">
-        <v>2</v>
+      <c r="D19" t="s" s="4">
+        <v>39</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" t="s" s="4">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" ht="20" customHeight="1">
@@ -1909,18 +1933,18 @@
         <v>18</v>
       </c>
       <c r="B20" t="s" s="4">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s" s="4">
         <v>35</v>
       </c>
-      <c r="D20" s="4">
-        <v>3</v>
+      <c r="D20" t="s" s="4">
+        <v>41</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" t="s" s="4">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" ht="20" customHeight="1">
@@ -1928,18 +1952,18 @@
         <v>19</v>
       </c>
       <c r="B21" t="s" s="4">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C21" t="s" s="4">
         <v>35</v>
       </c>
-      <c r="D21" s="4">
-        <v>4</v>
+      <c r="D21" t="s" s="4">
+        <v>43</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" t="s" s="4">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" ht="20" customHeight="1">
@@ -1947,18 +1971,18 @@
         <v>20</v>
       </c>
       <c r="B22" t="s" s="4">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C22" t="s" s="4">
         <v>35</v>
       </c>
-      <c r="D22" s="4">
-        <v>5</v>
+      <c r="D22" t="s" s="4">
+        <v>45</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" t="s" s="4">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" ht="20" customHeight="1">
@@ -1966,18 +1990,18 @@
         <v>21</v>
       </c>
       <c r="B23" t="s" s="4">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s" s="4">
         <v>35</v>
       </c>
-      <c r="D23" s="4">
-        <v>6</v>
+      <c r="D23" t="s" s="4">
+        <v>47</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" t="s" s="4">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" ht="20" customHeight="1">
@@ -1985,18 +2009,18 @@
         <v>22</v>
       </c>
       <c r="B24" t="s" s="4">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C24" t="s" s="4">
         <v>35</v>
       </c>
-      <c r="D24" s="4">
-        <v>7</v>
+      <c r="D24" t="s" s="4">
+        <v>49</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" t="s" s="4">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" ht="20" customHeight="1">
@@ -2004,18 +2028,18 @@
         <v>23</v>
       </c>
       <c r="B25" t="s" s="4">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C25" t="s" s="4">
         <v>35</v>
       </c>
-      <c r="D25" s="4">
-        <v>8</v>
+      <c r="D25" t="s" s="4">
+        <v>51</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" t="s" s="4">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" ht="20" customHeight="1">
@@ -2023,10 +2047,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="s" s="4">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s" s="4">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D26" s="4">
         <v>3</v>
@@ -2034,7 +2058,7 @@
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" t="s" s="4">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" ht="20" customHeight="1">
@@ -2042,10 +2066,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="s" s="4">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C27" t="s" s="4">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D27" s="4">
         <v>4</v>
@@ -2053,7 +2077,7 @@
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" t="s" s="4">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" ht="20" customHeight="1">
@@ -2061,10 +2085,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="s" s="4">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C28" t="s" s="4">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D28" s="4">
         <v>5</v>
@@ -2072,7 +2096,7 @@
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" t="s" s="4">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" ht="20" customHeight="1">
@@ -2080,10 +2104,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="s" s="4">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="C29" t="s" s="4">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D29" s="4">
         <v>6</v>
@@ -2091,7 +2115,7 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" t="s" s="4">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>